<commit_message>
Commiting HPLC data analysis
</commit_message>
<xml_diff>
--- a/HPLC/HPLC.xlsx
+++ b/HPLC/HPLC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Position 1" sheetId="1" state="visible" r:id="rId3"/>
@@ -17,6 +17,8 @@
     <sheet name="Area graphs" sheetId="7" state="visible" r:id="rId9"/>
     <sheet name="conc graphs" sheetId="8" state="visible" r:id="rId10"/>
     <sheet name="Red_increa graphs" sheetId="9" state="visible" r:id="rId11"/>
+    <sheet name="Export Pos 1" sheetId="10" state="visible" r:id="rId12"/>
+    <sheet name="Export Pos 2" sheetId="11" state="visible" r:id="rId13"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="36">
   <si>
     <t xml:space="preserve">Position 1</t>
   </si>
@@ -128,6 +130,15 @@
   <si>
     <t xml:space="preserve">propionic</t>
   </si>
+  <si>
+    <t xml:space="preserve">Lactate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acetate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Propionate</t>
+  </si>
 </sst>
 </file>
 
@@ -218,7 +229,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -260,6 +271,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -573,11 +592,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="77680708"/>
-        <c:axId val="29738301"/>
+        <c:axId val="34745462"/>
+        <c:axId val="30491729"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77680708"/>
+        <c:axId val="34745462"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -619,12 +638,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29738301"/>
+        <c:crossAx val="30491729"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="29738301"/>
+        <c:axId val="30491729"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -666,7 +685,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77680708"/>
+        <c:crossAx val="34745462"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -932,11 +951,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="44424836"/>
-        <c:axId val="29845490"/>
+        <c:axId val="33125013"/>
+        <c:axId val="34731026"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="44424836"/>
+        <c:axId val="33125013"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -978,12 +997,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29845490"/>
+        <c:crossAx val="34731026"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="29845490"/>
+        <c:axId val="34731026"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1025,7 +1044,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44424836"/>
+        <c:crossAx val="33125013"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1291,11 +1310,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="73039500"/>
-        <c:axId val="98649690"/>
+        <c:axId val="11745043"/>
+        <c:axId val="56605621"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73039500"/>
+        <c:axId val="11745043"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1337,12 +1356,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98649690"/>
+        <c:crossAx val="56605621"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="98649690"/>
+        <c:axId val="56605621"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1384,7 +1403,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73039500"/>
+        <c:crossAx val="11745043"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1650,11 +1669,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="73154649"/>
-        <c:axId val="52395089"/>
+        <c:axId val="95837182"/>
+        <c:axId val="45281255"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73154649"/>
+        <c:axId val="95837182"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1696,12 +1715,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52395089"/>
+        <c:crossAx val="45281255"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="52395089"/>
+        <c:axId val="45281255"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1743,7 +1762,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73154649"/>
+        <c:crossAx val="95837182"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2009,11 +2028,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="5577314"/>
-        <c:axId val="29917759"/>
+        <c:axId val="73990034"/>
+        <c:axId val="51576765"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="5577314"/>
+        <c:axId val="73990034"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2055,12 +2074,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29917759"/>
+        <c:crossAx val="51576765"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="29917759"/>
+        <c:axId val="51576765"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2102,7 +2121,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5577314"/>
+        <c:crossAx val="73990034"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2368,11 +2387,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="86155089"/>
-        <c:axId val="17703286"/>
+        <c:axId val="67426632"/>
+        <c:axId val="52670026"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86155089"/>
+        <c:axId val="67426632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2414,12 +2433,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17703286"/>
+        <c:crossAx val="52670026"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="17703286"/>
+        <c:axId val="52670026"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2461,7 +2480,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86155089"/>
+        <c:crossAx val="67426632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2727,11 +2746,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="5971766"/>
-        <c:axId val="10323750"/>
+        <c:axId val="35212849"/>
+        <c:axId val="7621798"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="5971766"/>
+        <c:axId val="35212849"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2773,12 +2792,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10323750"/>
+        <c:crossAx val="7621798"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="10323750"/>
+        <c:axId val="7621798"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2820,7 +2839,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5971766"/>
+        <c:crossAx val="35212849"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3086,11 +3105,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="6668352"/>
-        <c:axId val="14704244"/>
+        <c:axId val="2662609"/>
+        <c:axId val="17414032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="6668352"/>
+        <c:axId val="2662609"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3132,12 +3151,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14704244"/>
+        <c:crossAx val="17414032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="14704244"/>
+        <c:axId val="17414032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3179,7 +3198,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6668352"/>
+        <c:crossAx val="2662609"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3445,11 +3464,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="53250427"/>
-        <c:axId val="5906853"/>
+        <c:axId val="48292173"/>
+        <c:axId val="31922702"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53250427"/>
+        <c:axId val="48292173"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3491,12 +3510,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5906853"/>
+        <c:crossAx val="31922702"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="5906853"/>
+        <c:axId val="31922702"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3538,7 +3557,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53250427"/>
+        <c:crossAx val="48292173"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3804,11 +3823,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="24489218"/>
-        <c:axId val="15008160"/>
+        <c:axId val="44547534"/>
+        <c:axId val="45311466"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="24489218"/>
+        <c:axId val="44547534"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3850,12 +3869,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15008160"/>
+        <c:crossAx val="45311466"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="15008160"/>
+        <c:axId val="45311466"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3897,7 +3916,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="24489218"/>
+        <c:crossAx val="44547534"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4163,11 +4182,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="85553787"/>
-        <c:axId val="82860587"/>
+        <c:axId val="93849494"/>
+        <c:axId val="95987023"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85553787"/>
+        <c:axId val="93849494"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4209,12 +4228,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82860587"/>
+        <c:crossAx val="95987023"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82860587"/>
+        <c:axId val="95987023"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4256,7 +4275,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85553787"/>
+        <c:crossAx val="93849494"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4522,11 +4541,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="40507909"/>
-        <c:axId val="85233172"/>
+        <c:axId val="10545851"/>
+        <c:axId val="18099246"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="40507909"/>
+        <c:axId val="10545851"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4568,12 +4587,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85233172"/>
+        <c:crossAx val="18099246"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85233172"/>
+        <c:axId val="18099246"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4615,7 +4634,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40507909"/>
+        <c:crossAx val="10545851"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4881,11 +4900,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="28065038"/>
-        <c:axId val="36052957"/>
+        <c:axId val="40632435"/>
+        <c:axId val="56969826"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="28065038"/>
+        <c:axId val="40632435"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4927,12 +4946,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36052957"/>
+        <c:crossAx val="56969826"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="36052957"/>
+        <c:axId val="56969826"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4974,7 +4993,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28065038"/>
+        <c:crossAx val="40632435"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5240,11 +5259,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="42355556"/>
-        <c:axId val="32466758"/>
+        <c:axId val="82029377"/>
+        <c:axId val="30829594"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="42355556"/>
+        <c:axId val="82029377"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5286,12 +5305,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32466758"/>
+        <c:crossAx val="30829594"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="32466758"/>
+        <c:axId val="30829594"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5333,7 +5352,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42355556"/>
+        <c:crossAx val="82029377"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5599,11 +5618,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="33807053"/>
-        <c:axId val="62937768"/>
+        <c:axId val="8281420"/>
+        <c:axId val="72008012"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="33807053"/>
+        <c:axId val="8281420"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5645,12 +5664,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62937768"/>
+        <c:crossAx val="72008012"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="62937768"/>
+        <c:axId val="72008012"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5692,7 +5711,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="33807053"/>
+        <c:crossAx val="8281420"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5958,11 +5977,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="17096317"/>
-        <c:axId val="44528204"/>
+        <c:axId val="17714413"/>
+        <c:axId val="94904771"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="17096317"/>
+        <c:axId val="17714413"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6004,12 +6023,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44528204"/>
+        <c:crossAx val="94904771"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44528204"/>
+        <c:axId val="94904771"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6051,7 +6070,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17096317"/>
+        <c:crossAx val="17714413"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6208,11 +6227,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="35564205"/>
-        <c:axId val="92351750"/>
+        <c:axId val="42430955"/>
+        <c:axId val="99183791"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="35564205"/>
+        <c:axId val="42430955"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6254,7 +6273,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92351750"/>
+        <c:crossAx val="99183791"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6262,7 +6281,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92351750"/>
+        <c:axId val="99183791"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6304,7 +6323,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35564205"/>
+        <c:crossAx val="42430955"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6461,11 +6480,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="29013035"/>
-        <c:axId val="38382014"/>
+        <c:axId val="14712847"/>
+        <c:axId val="22555003"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="29013035"/>
+        <c:axId val="14712847"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6507,7 +6526,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38382014"/>
+        <c:crossAx val="22555003"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6515,7 +6534,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="38382014"/>
+        <c:axId val="22555003"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6557,7 +6576,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29013035"/>
+        <c:crossAx val="14712847"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6714,11 +6733,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="62786634"/>
-        <c:axId val="99045478"/>
+        <c:axId val="61588425"/>
+        <c:axId val="38600323"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="62786634"/>
+        <c:axId val="61588425"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6760,7 +6779,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99045478"/>
+        <c:crossAx val="38600323"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6768,7 +6787,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99045478"/>
+        <c:axId val="38600323"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6810,7 +6829,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62786634"/>
+        <c:crossAx val="61588425"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6967,11 +6986,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="75289014"/>
-        <c:axId val="45637903"/>
+        <c:axId val="64127883"/>
+        <c:axId val="18340154"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="75289014"/>
+        <c:axId val="64127883"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7013,7 +7032,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45637903"/>
+        <c:crossAx val="18340154"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7021,7 +7040,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45637903"/>
+        <c:axId val="18340154"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7063,7 +7082,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75289014"/>
+        <c:crossAx val="64127883"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7220,11 +7239,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="25872580"/>
-        <c:axId val="51074930"/>
+        <c:axId val="72024484"/>
+        <c:axId val="66987910"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="25872580"/>
+        <c:axId val="72024484"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7266,7 +7285,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51074930"/>
+        <c:crossAx val="66987910"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7274,7 +7293,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51074930"/>
+        <c:axId val="66987910"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7316,7 +7335,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25872580"/>
+        <c:crossAx val="72024484"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7473,11 +7492,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="19917132"/>
-        <c:axId val="51730935"/>
+        <c:axId val="46053816"/>
+        <c:axId val="13761516"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="19917132"/>
+        <c:axId val="46053816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7519,7 +7538,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51730935"/>
+        <c:crossAx val="13761516"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7527,7 +7546,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51730935"/>
+        <c:axId val="13761516"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7569,7 +7588,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19917132"/>
+        <c:crossAx val="46053816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7835,11 +7854,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="49419531"/>
-        <c:axId val="80820466"/>
+        <c:axId val="42149364"/>
+        <c:axId val="66133038"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="49419531"/>
+        <c:axId val="42149364"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7881,12 +7900,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80820466"/>
+        <c:crossAx val="66133038"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80820466"/>
+        <c:axId val="66133038"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7928,7 +7947,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49419531"/>
+        <c:crossAx val="42149364"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8246,11 +8265,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="67191111"/>
-        <c:axId val="81266199"/>
+        <c:axId val="85724111"/>
+        <c:axId val="1224411"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="67191111"/>
+        <c:axId val="85724111"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8292,12 +8311,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81266199"/>
+        <c:crossAx val="1224411"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81266199"/>
+        <c:axId val="1224411"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8339,7 +8358,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67191111"/>
+        <c:crossAx val="85724111"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8681,11 +8700,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="17184003"/>
-        <c:axId val="60687068"/>
+        <c:axId val="41870077"/>
+        <c:axId val="97955459"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="17184003"/>
+        <c:axId val="41870077"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8727,12 +8746,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60687068"/>
+        <c:crossAx val="97955459"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="60687068"/>
+        <c:axId val="97955459"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8774,7 +8793,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17184003"/>
+        <c:crossAx val="41870077"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9116,11 +9135,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="5966275"/>
-        <c:axId val="2401151"/>
+        <c:axId val="2461777"/>
+        <c:axId val="85712716"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="5966275"/>
+        <c:axId val="2461777"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9162,12 +9181,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2401151"/>
+        <c:crossAx val="85712716"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2401151"/>
+        <c:axId val="85712716"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9209,7 +9228,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5966275"/>
+        <c:crossAx val="2461777"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9551,11 +9570,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="91366345"/>
-        <c:axId val="9910091"/>
+        <c:axId val="10130450"/>
+        <c:axId val="38677733"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91366345"/>
+        <c:axId val="10130450"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9597,12 +9616,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9910091"/>
+        <c:crossAx val="38677733"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="9910091"/>
+        <c:axId val="38677733"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9644,7 +9663,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91366345"/>
+        <c:crossAx val="10130450"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9986,11 +10005,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="95491160"/>
-        <c:axId val="53105392"/>
+        <c:axId val="4483288"/>
+        <c:axId val="47279365"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95491160"/>
+        <c:axId val="4483288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10032,12 +10051,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53105392"/>
+        <c:crossAx val="47279365"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53105392"/>
+        <c:axId val="47279365"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10079,7 +10098,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95491160"/>
+        <c:crossAx val="4483288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10421,11 +10440,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="34355337"/>
-        <c:axId val="13384676"/>
+        <c:axId val="45640059"/>
+        <c:axId val="70926660"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="34355337"/>
+        <c:axId val="45640059"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10467,12 +10486,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13384676"/>
+        <c:crossAx val="70926660"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="13384676"/>
+        <c:axId val="70926660"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10514,7 +10533,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34355337"/>
+        <c:crossAx val="45640059"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10856,11 +10875,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="66113592"/>
-        <c:axId val="65112833"/>
+        <c:axId val="77572774"/>
+        <c:axId val="33527919"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="66113592"/>
+        <c:axId val="77572774"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10902,12 +10921,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65112833"/>
+        <c:crossAx val="33527919"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65112833"/>
+        <c:axId val="33527919"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10949,7 +10968,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66113592"/>
+        <c:crossAx val="77572774"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11291,11 +11310,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="2810441"/>
-        <c:axId val="50174145"/>
+        <c:axId val="50628402"/>
+        <c:axId val="36735350"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2810441"/>
+        <c:axId val="50628402"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11337,12 +11356,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50174145"/>
+        <c:crossAx val="36735350"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="50174145"/>
+        <c:axId val="36735350"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11384,7 +11403,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2810441"/>
+        <c:crossAx val="50628402"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11726,11 +11745,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="31427342"/>
-        <c:axId val="17627924"/>
+        <c:axId val="94319597"/>
+        <c:axId val="40736255"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="31427342"/>
+        <c:axId val="94319597"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11772,12 +11791,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17627924"/>
+        <c:crossAx val="40736255"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="17627924"/>
+        <c:axId val="40736255"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11819,7 +11838,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31427342"/>
+        <c:crossAx val="94319597"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12161,11 +12180,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="77767624"/>
-        <c:axId val="72269454"/>
+        <c:axId val="66436764"/>
+        <c:axId val="34176562"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77767624"/>
+        <c:axId val="66436764"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12207,12 +12226,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72269454"/>
+        <c:crossAx val="34176562"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72269454"/>
+        <c:axId val="34176562"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12254,7 +12273,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77767624"/>
+        <c:crossAx val="66436764"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12544,11 +12563,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="89369162"/>
-        <c:axId val="75660117"/>
+        <c:axId val="58922861"/>
+        <c:axId val="17311219"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="89369162"/>
+        <c:axId val="58922861"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12590,12 +12609,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75660117"/>
+        <c:crossAx val="17311219"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75660117"/>
+        <c:axId val="17311219"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12637,7 +12656,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89369162"/>
+        <c:crossAx val="58922861"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12955,11 +12974,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="22479861"/>
-        <c:axId val="64119837"/>
+        <c:axId val="42734996"/>
+        <c:axId val="61488075"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="22479861"/>
+        <c:axId val="42734996"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13001,12 +13020,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64119837"/>
+        <c:crossAx val="61488075"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64119837"/>
+        <c:axId val="61488075"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13048,7 +13067,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22479861"/>
+        <c:crossAx val="42734996"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13390,11 +13409,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="36983175"/>
-        <c:axId val="4955942"/>
+        <c:axId val="14664046"/>
+        <c:axId val="72046881"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="36983175"/>
+        <c:axId val="14664046"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13436,12 +13455,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4955942"/>
+        <c:crossAx val="72046881"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="4955942"/>
+        <c:axId val="72046881"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13483,7 +13502,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36983175"/>
+        <c:crossAx val="14664046"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13771,11 +13790,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="16270914"/>
-        <c:axId val="14853957"/>
+        <c:axId val="93029284"/>
+        <c:axId val="71689411"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="16270914"/>
+        <c:axId val="93029284"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13817,12 +13836,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14853957"/>
+        <c:crossAx val="71689411"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="14853957"/>
+        <c:axId val="71689411"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13864,7 +13883,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16270914"/>
+        <c:crossAx val="93029284"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14206,11 +14225,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="60648597"/>
-        <c:axId val="3595857"/>
+        <c:axId val="19806900"/>
+        <c:axId val="1218729"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="60648597"/>
+        <c:axId val="19806900"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14252,12 +14271,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3595857"/>
+        <c:crossAx val="1218729"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="3595857"/>
+        <c:axId val="1218729"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14299,7 +14318,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60648597"/>
+        <c:crossAx val="19806900"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14641,11 +14660,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="79747759"/>
-        <c:axId val="56997863"/>
+        <c:axId val="41421442"/>
+        <c:axId val="60696101"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="79747759"/>
+        <c:axId val="41421442"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14687,12 +14706,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56997863"/>
+        <c:crossAx val="60696101"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="56997863"/>
+        <c:axId val="60696101"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14734,7 +14753,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79747759"/>
+        <c:crossAx val="41421442"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15070,11 +15089,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="62339699"/>
-        <c:axId val="768159"/>
+        <c:axId val="55500340"/>
+        <c:axId val="21777744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="62339699"/>
+        <c:axId val="55500340"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15116,12 +15135,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="768159"/>
+        <c:crossAx val="21777744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="768159"/>
+        <c:axId val="21777744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15163,7 +15182,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62339699"/>
+        <c:crossAx val="55500340"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15499,11 +15518,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="59632826"/>
-        <c:axId val="29019838"/>
+        <c:axId val="14458686"/>
+        <c:axId val="24626751"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="59632826"/>
+        <c:axId val="14458686"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15545,12 +15564,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29019838"/>
+        <c:crossAx val="24626751"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="29019838"/>
+        <c:axId val="24626751"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15592,7 +15611,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59632826"/>
+        <c:crossAx val="14458686"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15928,11 +15947,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="94587013"/>
-        <c:axId val="16986772"/>
+        <c:axId val="17141080"/>
+        <c:axId val="60111256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="94587013"/>
+        <c:axId val="17141080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15974,12 +15993,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16986772"/>
+        <c:crossAx val="60111256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="16986772"/>
+        <c:axId val="60111256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16021,7 +16040,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94587013"/>
+        <c:crossAx val="17141080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -16357,11 +16376,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="9326611"/>
-        <c:axId val="90783435"/>
+        <c:axId val="84135058"/>
+        <c:axId val="31050629"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="9326611"/>
+        <c:axId val="84135058"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16403,12 +16422,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90783435"/>
+        <c:crossAx val="31050629"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90783435"/>
+        <c:axId val="31050629"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16450,7 +16469,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9326611"/>
+        <c:crossAx val="84135058"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -16738,11 +16757,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="88764844"/>
-        <c:axId val="66790313"/>
+        <c:axId val="88561292"/>
+        <c:axId val="5001132"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="88764844"/>
+        <c:axId val="88561292"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16784,12 +16803,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66790313"/>
+        <c:crossAx val="5001132"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="66790313"/>
+        <c:axId val="5001132"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16831,7 +16850,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88764844"/>
+        <c:crossAx val="88561292"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -17121,11 +17140,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="99894635"/>
-        <c:axId val="85837008"/>
+        <c:axId val="91423830"/>
+        <c:axId val="17924471"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99894635"/>
+        <c:axId val="91423830"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17167,12 +17186,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85837008"/>
+        <c:crossAx val="17924471"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85837008"/>
+        <c:axId val="17924471"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17214,7 +17233,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99894635"/>
+        <c:crossAx val="91423830"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -17526,11 +17545,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="35003284"/>
-        <c:axId val="46280192"/>
+        <c:axId val="79265502"/>
+        <c:axId val="62005608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="35003284"/>
+        <c:axId val="79265502"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17572,12 +17591,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46280192"/>
+        <c:crossAx val="62005608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="46280192"/>
+        <c:axId val="62005608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17619,7 +17638,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35003284"/>
+        <c:crossAx val="79265502"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -17909,11 +17928,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="29384163"/>
-        <c:axId val="69225253"/>
+        <c:axId val="96983157"/>
+        <c:axId val="41025789"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="29384163"/>
+        <c:axId val="96983157"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17955,12 +17974,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69225253"/>
+        <c:crossAx val="41025789"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69225253"/>
+        <c:axId val="41025789"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18002,7 +18021,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29384163"/>
+        <c:crossAx val="96983157"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -18268,11 +18287,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="97084268"/>
-        <c:axId val="91010641"/>
+        <c:axId val="97768859"/>
+        <c:axId val="70735883"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="97084268"/>
+        <c:axId val="97768859"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18314,12 +18333,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91010641"/>
+        <c:crossAx val="70735883"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91010641"/>
+        <c:axId val="70735883"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18361,7 +18380,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97084268"/>
+        <c:crossAx val="97768859"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -18627,11 +18646,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="5525757"/>
-        <c:axId val="71574003"/>
+        <c:axId val="56017252"/>
+        <c:axId val="15892430"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="5525757"/>
+        <c:axId val="56017252"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18673,12 +18692,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71574003"/>
+        <c:crossAx val="15892430"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71574003"/>
+        <c:axId val="15892430"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18720,7 +18739,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5525757"/>
+        <c:crossAx val="56017252"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -18986,11 +19005,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="94122246"/>
-        <c:axId val="95014938"/>
+        <c:axId val="11912647"/>
+        <c:axId val="7407175"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="94122246"/>
+        <c:axId val="11912647"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19032,12 +19051,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95014938"/>
+        <c:crossAx val="7407175"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95014938"/>
+        <c:axId val="7407175"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19079,7 +19098,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94122246"/>
+        <c:crossAx val="11912647"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -19118,9 +19137,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>114120</xdr:colOff>
+      <xdr:colOff>113760</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>50040</xdr:rowOff>
+      <xdr:rowOff>49680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -19129,7 +19148,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="16036920" y="3974760"/>
-        <a:ext cx="5011920" cy="2742840"/>
+        <a:ext cx="5011560" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -19148,9 +19167,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>87480</xdr:colOff>
+      <xdr:colOff>87120</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>72000</xdr:rowOff>
+      <xdr:rowOff>71640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -19159,7 +19178,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="16010280" y="948960"/>
-        <a:ext cx="5011920" cy="2742480"/>
+        <a:ext cx="5011560" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -19178,9 +19197,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>36</xdr:col>
-      <xdr:colOff>567360</xdr:colOff>
+      <xdr:colOff>567000</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>80280</xdr:rowOff>
+      <xdr:rowOff>79920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -19189,7 +19208,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="21169800" y="957240"/>
-        <a:ext cx="4968360" cy="2742480"/>
+        <a:ext cx="4968000" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -19208,9 +19227,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>335880</xdr:colOff>
+      <xdr:colOff>335520</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>47160</xdr:rowOff>
+      <xdr:rowOff>46800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -19219,7 +19238,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="4389480" y="6067440"/>
-        <a:ext cx="4959720" cy="2742840"/>
+        <a:ext cx="4959360" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -19238,9 +19257,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>297720</xdr:colOff>
+      <xdr:colOff>297360</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>132480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -19249,7 +19268,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="4305240" y="3105360"/>
-        <a:ext cx="5005800" cy="2742480"/>
+        <a:ext cx="5005440" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -19268,9 +19287,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>192600</xdr:colOff>
+      <xdr:colOff>192240</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>94680</xdr:rowOff>
+      <xdr:rowOff>94320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -19279,7 +19298,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="9508680" y="3067200"/>
-        <a:ext cx="4995720" cy="2742480"/>
+        <a:ext cx="4995360" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -19298,9 +19317,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>468720</xdr:colOff>
+      <xdr:colOff>468360</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>37440</xdr:rowOff>
+      <xdr:rowOff>37080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -19309,7 +19328,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="9827640" y="6057720"/>
-        <a:ext cx="4952880" cy="2742840"/>
+        <a:ext cx="4952520" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -19328,9 +19347,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
-      <xdr:colOff>156240</xdr:colOff>
+      <xdr:colOff>155880</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>4320</xdr:rowOff>
+      <xdr:rowOff>3960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -19339,7 +19358,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="22049640" y="4310280"/>
-        <a:ext cx="5002200" cy="2742480"/>
+        <a:ext cx="5001840" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -19358,9 +19377,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>408960</xdr:colOff>
+      <xdr:colOff>408600</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>23400</xdr:rowOff>
+      <xdr:rowOff>23040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -19369,7 +19388,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="16384320" y="6996240"/>
-        <a:ext cx="4959360" cy="2742840"/>
+        <a:ext cx="4959000" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -19388,9 +19407,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>661320</xdr:colOff>
+      <xdr:colOff>660960</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>113760</xdr:rowOff>
+      <xdr:rowOff>113400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -19399,7 +19418,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="21882960" y="7467840"/>
-        <a:ext cx="5011560" cy="2742480"/>
+        <a:ext cx="5011200" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -19418,9 +19437,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>275760</xdr:colOff>
+      <xdr:colOff>275400</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -19429,7 +19448,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="10909440" y="9429840"/>
-        <a:ext cx="5002560" cy="2742840"/>
+        <a:ext cx="5002200" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -19448,9 +19467,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>315360</xdr:colOff>
+      <xdr:colOff>315000</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>163080</xdr:rowOff>
+      <xdr:rowOff>162720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -19459,7 +19478,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="16231680" y="10374480"/>
-        <a:ext cx="5018400" cy="2742480"/>
+        <a:ext cx="5018040" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -19478,9 +19497,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>609120</xdr:colOff>
+      <xdr:colOff>608760</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>146880</xdr:rowOff>
+      <xdr:rowOff>146520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -19489,7 +19508,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="5325120" y="9405720"/>
-        <a:ext cx="4959360" cy="2742840"/>
+        <a:ext cx="4959000" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -19513,9 +19532,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>114120</xdr:colOff>
+      <xdr:colOff>113760</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>50040</xdr:rowOff>
+      <xdr:rowOff>49680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -19524,7 +19543,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="15827400" y="3974760"/>
-        <a:ext cx="5011920" cy="2742840"/>
+        <a:ext cx="5011560" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -19543,9 +19562,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>87480</xdr:colOff>
+      <xdr:colOff>87120</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>72000</xdr:rowOff>
+      <xdr:rowOff>71640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -19554,7 +19573,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="15800760" y="948960"/>
-        <a:ext cx="5011920" cy="2742480"/>
+        <a:ext cx="5011560" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -19573,9 +19592,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>36</xdr:col>
-      <xdr:colOff>567360</xdr:colOff>
+      <xdr:colOff>567000</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>80280</xdr:rowOff>
+      <xdr:rowOff>79920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -19584,7 +19603,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="20960280" y="957240"/>
-        <a:ext cx="4968360" cy="2742480"/>
+        <a:ext cx="4968000" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -19603,9 +19622,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>213480</xdr:colOff>
+      <xdr:colOff>213120</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>155880</xdr:rowOff>
+      <xdr:rowOff>155520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -19614,7 +19633,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="5994720" y="6366960"/>
-        <a:ext cx="5009400" cy="2742480"/>
+        <a:ext cx="5009040" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -19633,9 +19652,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>297720</xdr:colOff>
+      <xdr:colOff>297360</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>132480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -19644,7 +19663,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="4095720" y="3105360"/>
-        <a:ext cx="5005800" cy="2742480"/>
+        <a:ext cx="5005440" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -19663,9 +19682,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>192960</xdr:colOff>
+      <xdr:colOff>192600</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>94680</xdr:rowOff>
+      <xdr:rowOff>94320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -19674,7 +19693,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="9299160" y="3067200"/>
-        <a:ext cx="4995720" cy="2742480"/>
+        <a:ext cx="4995360" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -19693,9 +19712,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>346680</xdr:colOff>
+      <xdr:colOff>346320</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>78480</xdr:rowOff>
+      <xdr:rowOff>78120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -19704,7 +19723,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="11482920" y="6670440"/>
-        <a:ext cx="4952880" cy="2742480"/>
+        <a:ext cx="4952520" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -19723,9 +19742,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
-      <xdr:colOff>156600</xdr:colOff>
+      <xdr:colOff>156240</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>4320</xdr:rowOff>
+      <xdr:rowOff>3960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -19734,7 +19753,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="21840120" y="4310280"/>
-        <a:ext cx="5002200" cy="2742480"/>
+        <a:ext cx="5001840" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -19753,9 +19772,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>502560</xdr:colOff>
+      <xdr:colOff>502200</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>140760</xdr:rowOff>
+      <xdr:rowOff>140400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -19764,7 +19783,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="18252720" y="7304040"/>
-        <a:ext cx="4961880" cy="2742840"/>
+        <a:ext cx="4961520" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -19783,9 +19802,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>248040</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>21240</xdr:rowOff>
+      <xdr:rowOff>20880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -19794,7 +19813,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="571680" y="6422760"/>
-        <a:ext cx="5168880" cy="2742480"/>
+        <a:ext cx="5168520" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -19818,9 +19837,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>427680</xdr:colOff>
+      <xdr:colOff>427320</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>123120</xdr:rowOff>
+      <xdr:rowOff>122760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -19829,7 +19848,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="6993360" y="237960"/>
-        <a:ext cx="5202000" cy="2742840"/>
+        <a:ext cx="5201640" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -19848,9 +19867,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>15120</xdr:colOff>
+      <xdr:colOff>14760</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>12240</xdr:rowOff>
+      <xdr:rowOff>11880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -19859,7 +19878,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="12541320" y="317520"/>
-        <a:ext cx="5202360" cy="2742840"/>
+        <a:ext cx="5202000" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -19878,9 +19897,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>364320</xdr:colOff>
+      <xdr:colOff>363960</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>123120</xdr:rowOff>
+      <xdr:rowOff>122760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -19889,7 +19908,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="6930000" y="3286080"/>
-        <a:ext cx="5202000" cy="2742480"/>
+        <a:ext cx="5201640" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -19908,9 +19927,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>364320</xdr:colOff>
+      <xdr:colOff>363960</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>59760</xdr:rowOff>
+      <xdr:rowOff>59400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -19919,7 +19938,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="12890520" y="3413160"/>
-        <a:ext cx="5202360" cy="2742480"/>
+        <a:ext cx="5202000" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -19938,9 +19957,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>491400</xdr:colOff>
+      <xdr:colOff>491040</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>43920</xdr:rowOff>
+      <xdr:rowOff>43560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -19949,7 +19968,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="18316080" y="349200"/>
-        <a:ext cx="5202360" cy="2742840"/>
+        <a:ext cx="5202000" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -19968,9 +19987,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>173880</xdr:colOff>
+      <xdr:colOff>173520</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>12240</xdr:rowOff>
+      <xdr:rowOff>11880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -19979,7 +19998,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="12700080" y="6413760"/>
-        <a:ext cx="5202360" cy="2742480"/>
+        <a:ext cx="5202000" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -20003,9 +20022,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>380520</xdr:colOff>
+      <xdr:colOff>380160</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>4320</xdr:rowOff>
+      <xdr:rowOff>3960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -20014,7 +20033,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="738720" y="2976840"/>
-        <a:ext cx="4940280" cy="2742480"/>
+        <a:ext cx="4939920" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -20033,9 +20052,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>266040</xdr:colOff>
+      <xdr:colOff>265680</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -20044,7 +20063,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="5870160" y="2953080"/>
-        <a:ext cx="4992840" cy="2742480"/>
+        <a:ext cx="4992480" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -20063,9 +20082,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>437400</xdr:colOff>
+      <xdr:colOff>437040</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>84960</xdr:rowOff>
+      <xdr:rowOff>84600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -20074,7 +20093,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="11297520" y="2867040"/>
-        <a:ext cx="5086800" cy="2742480"/>
+        <a:ext cx="5086440" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -20093,9 +20112,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>323280</xdr:colOff>
+      <xdr:colOff>322920</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>123120</xdr:rowOff>
+      <xdr:rowOff>122760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -20104,7 +20123,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="11130480" y="47520"/>
-        <a:ext cx="5139720" cy="2742480"/>
+        <a:ext cx="5139360" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -20123,9 +20142,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>563760</xdr:colOff>
+      <xdr:colOff>563400</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>123120</xdr:rowOff>
+      <xdr:rowOff>122760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -20134,7 +20153,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="912600" y="6143400"/>
-        <a:ext cx="4949640" cy="2742840"/>
+        <a:ext cx="4949280" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -20153,9 +20172,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>920880</xdr:colOff>
+      <xdr:colOff>920520</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>75600</xdr:rowOff>
+      <xdr:rowOff>75240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -20164,7 +20183,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="7285320" y="6477120"/>
-        <a:ext cx="4894920" cy="2742480"/>
+        <a:ext cx="4894560" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -20183,9 +20202,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>51840</xdr:colOff>
+      <xdr:colOff>51480</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>146880</xdr:rowOff>
+      <xdr:rowOff>146520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -20194,7 +20213,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="12937320" y="6357960"/>
-        <a:ext cx="5048280" cy="2742480"/>
+        <a:ext cx="5047920" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -20218,9 +20237,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>380520</xdr:colOff>
+      <xdr:colOff>380160</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>4320</xdr:rowOff>
+      <xdr:rowOff>3960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -20229,7 +20248,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="738720" y="2976840"/>
-        <a:ext cx="4940280" cy="2742480"/>
+        <a:ext cx="4939920" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -20248,9 +20267,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>266040</xdr:colOff>
+      <xdr:colOff>265680</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -20259,7 +20278,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="5870160" y="2953080"/>
-        <a:ext cx="4992840" cy="2742480"/>
+        <a:ext cx="4992480" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -20278,9 +20297,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>437400</xdr:colOff>
+      <xdr:colOff>437040</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>84960</xdr:rowOff>
+      <xdr:rowOff>84600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -20289,7 +20308,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="11297520" y="2867040"/>
-        <a:ext cx="5086800" cy="2742480"/>
+        <a:ext cx="5086440" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -20308,9 +20327,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>323280</xdr:colOff>
+      <xdr:colOff>322920</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>123120</xdr:rowOff>
+      <xdr:rowOff>122760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -20319,7 +20338,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="11130480" y="47520"/>
-        <a:ext cx="5139720" cy="2742480"/>
+        <a:ext cx="5139360" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -20338,9 +20357,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>563760</xdr:colOff>
+      <xdr:colOff>563400</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>123120</xdr:rowOff>
+      <xdr:rowOff>122760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -20349,7 +20368,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="912600" y="6143400"/>
-        <a:ext cx="4949640" cy="2742840"/>
+        <a:ext cx="4949280" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -20368,9 +20387,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>920880</xdr:colOff>
+      <xdr:colOff>920520</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>75600</xdr:rowOff>
+      <xdr:rowOff>75240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -20379,7 +20398,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="7285320" y="6477120"/>
-        <a:ext cx="4894920" cy="2742480"/>
+        <a:ext cx="4894560" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -20398,9 +20417,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>51840</xdr:colOff>
+      <xdr:colOff>51480</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>146880</xdr:rowOff>
+      <xdr:rowOff>146520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -20409,7 +20428,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="12937320" y="6357960"/>
-        <a:ext cx="5048280" cy="2742480"/>
+        <a:ext cx="5047920" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -20433,9 +20452,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>380520</xdr:colOff>
+      <xdr:colOff>380160</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>4320</xdr:rowOff>
+      <xdr:rowOff>3960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -20444,7 +20463,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="738720" y="2976840"/>
-        <a:ext cx="4940280" cy="2742480"/>
+        <a:ext cx="4939920" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -20463,9 +20482,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>266040</xdr:colOff>
+      <xdr:colOff>265680</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -20474,7 +20493,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="5870160" y="2953080"/>
-        <a:ext cx="4992840" cy="2742480"/>
+        <a:ext cx="4992480" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -20493,9 +20512,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>437400</xdr:colOff>
+      <xdr:colOff>437040</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>84960</xdr:rowOff>
+      <xdr:rowOff>84600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -20504,7 +20523,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="11297520" y="2867040"/>
-        <a:ext cx="5086800" cy="2742480"/>
+        <a:ext cx="5086440" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -20523,9 +20542,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>323280</xdr:colOff>
+      <xdr:colOff>322920</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>123120</xdr:rowOff>
+      <xdr:rowOff>122760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -20534,7 +20553,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="11130480" y="47520"/>
-        <a:ext cx="5139720" cy="2742480"/>
+        <a:ext cx="5139360" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -20553,9 +20572,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>563760</xdr:colOff>
+      <xdr:colOff>563400</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>123120</xdr:rowOff>
+      <xdr:rowOff>122760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -20564,7 +20583,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="912600" y="6143400"/>
-        <a:ext cx="4949640" cy="2742840"/>
+        <a:ext cx="4949280" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -20583,9 +20602,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>920880</xdr:colOff>
+      <xdr:colOff>920520</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>75600</xdr:rowOff>
+      <xdr:rowOff>75240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -20594,7 +20613,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="7285320" y="6477120"/>
-        <a:ext cx="4894920" cy="2742480"/>
+        <a:ext cx="4894560" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -20613,9 +20632,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>51840</xdr:colOff>
+      <xdr:colOff>51480</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>146880</xdr:rowOff>
+      <xdr:rowOff>146520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -20624,7 +20643,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="12937320" y="6357960"/>
-        <a:ext cx="5048280" cy="2742480"/>
+        <a:ext cx="5047920" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -20816,15 +20835,15 @@
   </sheetPr>
   <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q15" activeCellId="0" sqref="Q15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.62109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.35"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21867,6 +21886,990 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H20"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="n">
+        <v>258889</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>376900</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>783451</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>1664.23022</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>734.13501</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>525.50177</v>
+      </c>
+      <c r="H2" s="4" t="n">
+        <v>31624.1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="n">
+        <v>236229</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <v>337424</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>700292</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>1323.98901</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>720.08173</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>474.34052</v>
+      </c>
+      <c r="H3" s="4" t="n">
+        <v>18582.1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="n">
+        <v>278513</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>336926</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>646723</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>1302.66394</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>592.94244</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>451.06616</v>
+      </c>
+      <c r="H4" s="4" t="n">
+        <v>16218.6</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="n">
+        <v>274047</v>
+      </c>
+      <c r="C5" s="4" t="n">
+        <v>343269</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>640104</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>1286.83582</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>584.00891</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>451.36359</v>
+      </c>
+      <c r="H5" s="4" t="n">
+        <v>15520.3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="n">
+        <v>274373</v>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>357983</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>665690</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>1287.08752</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>594.7854</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>458.21854</v>
+      </c>
+      <c r="H6" s="4" t="n">
+        <v>14994.9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="n">
+        <v>279218</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>366695</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>664788</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>1281.9126</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>585.75012</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>466.4223</v>
+      </c>
+      <c r="H7" s="4" t="n">
+        <v>14571.4</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="n">
+        <v>235483</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>320000</v>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>555761</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>1133.43481</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>532.49994</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>419.74509</v>
+      </c>
+      <c r="H8" s="4" t="n">
+        <v>18350.6</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="B9" s="4" t="n">
+        <v>160820</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>8263.26855</v>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>546831</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>1508.52087</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>685.29639</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>599.16266</v>
+      </c>
+      <c r="H9" s="4" t="n">
+        <v>74898.7</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="B10" s="4" t="n">
+        <v>34326.1</v>
+      </c>
+      <c r="C10" s="4" t="n">
+        <v>17366.5</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>497387.2</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>1855.09375</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>762.00916</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>618.21094</v>
+      </c>
+      <c r="H10" s="4" t="n">
+        <v>76461.8</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="B11" s="4" t="n">
+        <v>20814.7</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>424911.2</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>1625.85071</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>702.23755</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>562.25879</v>
+      </c>
+      <c r="H11" s="4" t="n">
+        <v>60774.9</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="n">
+        <v>46</v>
+      </c>
+      <c r="B12" s="4" t="n">
+        <v>12225.3</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>424479.8</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>1546.89233</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>1083.46765</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>679.21783</v>
+      </c>
+      <c r="H12" s="4" t="n">
+        <v>55513.7</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="n">
+        <v>48</v>
+      </c>
+      <c r="B13" s="4" t="n">
+        <v>12174.6</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>437426.3</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>1545.38989</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>1161.0957</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>708.0155</v>
+      </c>
+      <c r="H13" s="4" t="n">
+        <v>63099.3</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="B14" s="4" t="n">
+        <v>14629.7</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>423957.4</v>
+      </c>
+      <c r="E14" s="4" t="n">
+        <v>1468.83154</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>1200.20569</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>724.4881</v>
+      </c>
+      <c r="H14" s="4" t="n">
+        <v>54020.3</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>378496.3</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>1201.35999</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>1390.53125</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>752.79211</v>
+      </c>
+      <c r="H15" s="4" t="n">
+        <v>45354.9</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="n">
+        <v>72</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>351582</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>1095.57202</v>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>1211.87817</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>704.30536</v>
+      </c>
+      <c r="H16" s="4" t="n">
+        <v>32821.5</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="n">
+        <v>74</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>396411.9</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>1191.29431</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>1480.43628</v>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>811.94141</v>
+      </c>
+      <c r="H17" s="4" t="n">
+        <v>43933.2</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="n">
+        <v>94</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>401889.4</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>941.83917</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>1763.89075</v>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>917.44592</v>
+      </c>
+      <c r="H18" s="4" t="n">
+        <v>36192.5</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="n">
+        <v>96</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>422100.1</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>936.25366</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>1862.53564</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>976.53821</v>
+      </c>
+      <c r="H19" s="4" t="n">
+        <v>33870.4</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="n">
+        <v>98</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>375159.5</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>799.48657</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>1708.92297</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>886.84436</v>
+      </c>
+      <c r="H20" s="4" t="n">
+        <v>31918.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="n">
+        <v>183496</v>
+      </c>
+      <c r="C2" s="8" t="n">
+        <v>268392</v>
+      </c>
+      <c r="D2" s="8" t="n">
+        <v>579738</v>
+      </c>
+      <c r="E2" s="9" t="n">
+        <v>1184.76611</v>
+      </c>
+      <c r="F2" s="9" t="n">
+        <v>562.10938</v>
+      </c>
+      <c r="G2" s="9" t="n">
+        <v>401.0654</v>
+      </c>
+      <c r="H2" s="8" t="n">
+        <v>16534.5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8" t="n">
+        <v>155841</v>
+      </c>
+      <c r="C3" s="8" t="n">
+        <v>227343</v>
+      </c>
+      <c r="D3" s="8" t="n">
+        <v>476364</v>
+      </c>
+      <c r="E3" s="9" t="n">
+        <v>982.81</v>
+      </c>
+      <c r="F3" s="9" t="n">
+        <v>473.16138</v>
+      </c>
+      <c r="G3" s="9" t="n">
+        <v>344.07239</v>
+      </c>
+      <c r="H3" s="8" t="n">
+        <v>13800.3</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>239669</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>320764</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>568859</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>1173.35742</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>553.00726</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>432.27405</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>15604.9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>203833</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>383357</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>574617</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>1209.14966</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>617.99353</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>550.29474</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>23240.7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="B6" s="8" t="n">
+        <v>144708</v>
+      </c>
+      <c r="C6" s="8" t="n">
+        <v>259343</v>
+      </c>
+      <c r="D6" s="8" t="n">
+        <v>513330</v>
+      </c>
+      <c r="E6" s="8" t="n">
+        <v>1159.86719</v>
+      </c>
+      <c r="F6" s="8" t="n">
+        <v>559.60663</v>
+      </c>
+      <c r="G6" s="8" t="n">
+        <v>529.77484</v>
+      </c>
+      <c r="H6" s="8" t="n">
+        <v>25930.9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="B7" s="8" t="n">
+        <v>129945</v>
+      </c>
+      <c r="C7" s="8" t="n">
+        <v>15283.2</v>
+      </c>
+      <c r="D7" s="8" t="n">
+        <v>463542</v>
+      </c>
+      <c r="E7" s="10" t="n">
+        <v>1371.60706</v>
+      </c>
+      <c r="F7" s="10" t="n">
+        <v>650.3208</v>
+      </c>
+      <c r="G7" s="10" t="n">
+        <v>571.0752</v>
+      </c>
+      <c r="H7" s="8" t="n">
+        <v>63526.2</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="n">
+        <v>46</v>
+      </c>
+      <c r="B8" s="8" t="n">
+        <v>7675.50342</v>
+      </c>
+      <c r="C8" s="8" t="n">
+        <v>13411.4</v>
+      </c>
+      <c r="D8" s="8" t="n">
+        <v>443389.5</v>
+      </c>
+      <c r="E8" s="8" t="n">
+        <v>1902.00342</v>
+      </c>
+      <c r="F8" s="8" t="n">
+        <v>845.53979</v>
+      </c>
+      <c r="G8" s="8" t="n">
+        <v>704.00055</v>
+      </c>
+      <c r="H8" s="8" t="n">
+        <v>73063.1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="11" t="n">
+        <v>48</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>8203.24512</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="8" t="n">
+        <v>443390.5</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>1825.60193</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>820.35632</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>692.75458</v>
+      </c>
+      <c r="H9" s="12" t="n">
+        <v>53261.8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="11" t="n">
+        <v>50</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>7814.33936</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="8" t="n">
+        <v>443391.5</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>1852.28723</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>843.15344</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>706.6897</v>
+      </c>
+      <c r="H10" s="12" t="n">
+        <v>84813.5</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="11" t="n">
+        <v>70</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="8" t="n">
+        <v>443392.5</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>1326.04919</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>809.62665</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>704.36536</v>
+      </c>
+      <c r="H11" s="12" t="n">
+        <v>44057</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="11" t="n">
+        <v>72</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="8" t="n">
+        <v>443393.5</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>1429.47583</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>926.9115</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>762.31635</v>
+      </c>
+      <c r="H12" s="12" t="n">
+        <v>49254.1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="11" t="n">
+        <v>74</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="8" t="n">
+        <v>443394.5</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>1542.21924</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>1096.56055</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>855.97583</v>
+      </c>
+      <c r="H13" s="12" t="n">
+        <v>58391.1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="11" t="n">
+        <v>94</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="8" t="n">
+        <v>443395.5</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>1106.44482</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>1276.96765</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>945.51862</v>
+      </c>
+      <c r="H14" s="12" t="n">
+        <v>53926.6</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="11" t="n">
+        <v>96</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="8" t="n">
+        <v>443396.5</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>938.74713</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>1178.45557</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>861.97796</v>
+      </c>
+      <c r="H15" s="12" t="n">
+        <v>41139.1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="11" t="n">
+        <v>98</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="8" t="n">
+        <v>443397.5</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>944.94617</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>1256.91504</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>920.44464</v>
+      </c>
+      <c r="H16" s="12" t="n">
+        <v>47208.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -21874,7 +22877,7 @@
   </sheetPr>
   <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O7" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -22932,7 +23935,7 @@
   <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="N10" activeCellId="0" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.62109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23279,7 +24282,7 @@
   </sheetPr>
   <dimension ref="A1:AO30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="AB47" activeCellId="0" sqref="AB47"/>
     </sheetView>
   </sheetViews>
@@ -23890,7 +24893,7 @@
   </sheetPr>
   <dimension ref="A1:W38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
     </sheetView>
   </sheetViews>
@@ -25848,7 +26851,7 @@
       </c>
       <c r="B18" s="1" t="n">
         <f aca="false">(($B$3-B4)/$B$3)*100</f>
-        <v>9.6816926708962</v>
+        <v>9.68169267089595</v>
       </c>
       <c r="C18" s="1" t="n">
         <f aca="false">(($C$3-C4)/$C$3)*100</f>
@@ -25856,7 +26859,7 @@
       </c>
       <c r="D18" s="1" t="n">
         <f aca="false">(($D$3-D4)/$D$3)*100</f>
-        <v>10.5477247042145</v>
+        <v>10.5477247042146</v>
       </c>
       <c r="E18" s="1" t="n">
         <f aca="false">(($E$3-E4)/$E$3)*100</f>
@@ -25864,7 +26867,7 @@
       </c>
       <c r="F18" s="1" t="n">
         <f aca="false">(($F$3-F4)/$F$3)*100</f>
-        <v>10.790560564214</v>
+        <v>10.7905605642141</v>
       </c>
       <c r="G18" s="1" t="n">
         <f aca="false">(($G$3-G4)/$G$3)*100</f>
@@ -25901,7 +26904,7 @@
       </c>
       <c r="B19" s="1" t="n">
         <f aca="false">(($B$3-B5)/$B$3)*100</f>
-        <v>-8.38453384702854</v>
+        <v>-8.38453384702855</v>
       </c>
       <c r="D19" s="1" t="n">
         <f aca="false">(($D$3-D5)/$D$3)*100</f>
@@ -25909,23 +26912,23 @@
       </c>
       <c r="F19" s="1" t="n">
         <f aca="false">(($F$3-F5)/$F$3)*100</f>
-        <v>17.7415765560415</v>
+        <v>17.7415765560417</v>
       </c>
       <c r="H19" s="1" t="n">
         <f aca="false">((H4-$H$3)/$H$3)*100</f>
-        <v>-20.4559830672872</v>
+        <v>-20.4559830672874</v>
       </c>
       <c r="I19" s="1" t="n">
         <f aca="false">((I4-$I$3)/$I$3)*100</f>
-        <v>-17.0596907912877</v>
+        <v>-17.0596907912878</v>
       </c>
       <c r="J19" s="1" t="n">
         <f aca="false">((J4-$J$3)/$J$3)*100</f>
-        <v>-1.9124825754133</v>
+        <v>-1.91248257541317</v>
       </c>
       <c r="K19" s="1" t="n">
         <f aca="false">((K4-$K$3)/$K$3)*100</f>
-        <v>-15.8047427060543</v>
+        <v>-15.8047427060541</v>
       </c>
       <c r="N19" s="1" t="n">
         <f aca="false">((N4-$N$3)/$N$3)*100</f>
@@ -25942,19 +26945,19 @@
       </c>
       <c r="B20" s="1" t="n">
         <f aca="false">(($B$3-B6)/$B$3)*100</f>
-        <v>-6.47639441771599</v>
+        <v>-6.47639441771598</v>
       </c>
       <c r="D20" s="1" t="n">
         <f aca="false">(($D$3-D6)/$D$3)*100</f>
-        <v>8.98597957056031</v>
+        <v>8.98597957056041</v>
       </c>
       <c r="F20" s="1" t="n">
         <f aca="false">(($F$3-F6)/$F$3)*100</f>
-        <v>18.6004459553192</v>
+        <v>18.6004459553195</v>
       </c>
       <c r="H20" s="1" t="n">
         <f aca="false">((H5-$H$3)/$H$3)*100</f>
-        <v>-21.7380889909897</v>
+        <v>-21.7380889909899</v>
       </c>
       <c r="J20" s="1" t="n">
         <f aca="false">((J5-$J$3)/$J$3)*100</f>
@@ -25971,19 +26974,19 @@
       </c>
       <c r="B21" s="1" t="n">
         <f aca="false">(($B$3-B7)/$B$3)*100</f>
-        <v>-6.61568090539085</v>
+        <v>-6.61568090539097</v>
       </c>
       <c r="D21" s="1" t="n">
         <f aca="false">(($D$3-D7)/$D$3)*100</f>
-        <v>5.05449661134932</v>
+        <v>5.05449661134936</v>
       </c>
       <c r="F21" s="1" t="n">
         <f aca="false">(($F$3-F7)/$F$3)*100</f>
-        <v>15.2804531391961</v>
+        <v>15.2804531391962</v>
       </c>
       <c r="H21" s="1" t="n">
         <f aca="false">((H6-$H$3)/$H$3)*100</f>
-        <v>-22.6897072699953</v>
+        <v>-22.6897072699955</v>
       </c>
       <c r="J21" s="1" t="n">
         <f aca="false">((J6-$J$3)/$J$3)*100</f>
@@ -26000,15 +27003,15 @@
       </c>
       <c r="B22" s="1" t="n">
         <f aca="false">(($B$3-B8)/$B$3)*100</f>
-        <v>-8.68575155810453</v>
+        <v>-8.68575155810477</v>
       </c>
       <c r="C22" s="1" t="n">
         <f aca="false">(($C$3-C8)/$C$3)*100</f>
-        <v>-35.4053122162973</v>
+        <v>-35.4053122162971</v>
       </c>
       <c r="D22" s="1" t="n">
         <f aca="false">(($D$3-D8)/$D$3)*100</f>
-        <v>2.72670814182058</v>
+        <v>2.72670814182057</v>
       </c>
       <c r="E22" s="1" t="n">
         <f aca="false">(($E$3-E8)/$E$3)*100</f>
@@ -26016,15 +27019,15 @@
       </c>
       <c r="F22" s="1" t="n">
         <f aca="false">(($F$3-F8)/$F$3)*100</f>
-        <v>15.3974950183544</v>
+        <v>15.3974950183545</v>
       </c>
       <c r="G22" s="1" t="n">
         <f aca="false">(($G$3-G8)/$G$3)*100</f>
-        <v>1.9188596359425</v>
+        <v>1.9188596359423</v>
       </c>
       <c r="H22" s="1" t="n">
         <f aca="false">((H7-$H$3)/$H$3)*100</f>
-        <v>-22.6745745618262</v>
+        <v>-22.6745745618263</v>
       </c>
       <c r="J22" s="1" t="n">
         <f aca="false">((J7-$J$3)/$J$3)*100</f>
@@ -26032,7 +27035,7 @@
       </c>
       <c r="N22" s="1" t="n">
         <f aca="false">((N7-$N$3)/$N$3)*100</f>
-        <v>-72.7797092964517</v>
+        <v>-72.7797092964516</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26041,23 +27044,23 @@
       </c>
       <c r="B23" s="1" t="n">
         <f aca="false">(($B$3-B9)/$B$3)*100</f>
-        <v>10.0004280077227</v>
+        <v>10.0004280077225</v>
       </c>
       <c r="D23" s="1" t="n">
         <f aca="false">(($D$3-D9)/$D$3)*100</f>
-        <v>15.203301643272</v>
+        <v>15.2033016432721</v>
       </c>
       <c r="F23" s="1" t="n">
         <f aca="false">(($F$3-F9)/$F$3)*100</f>
-        <v>29.544640205701</v>
+        <v>29.5446402057011</v>
       </c>
       <c r="H23" s="1" t="n">
         <f aca="false">((H8-$H$3)/$H$3)*100</f>
-        <v>-22.9857011178791</v>
+        <v>-22.9857011178792</v>
       </c>
       <c r="I23" s="1" t="n">
         <f aca="false">((I8-$I$3)/$I$3)*100</f>
-        <v>-0.963717927294474</v>
+        <v>-0.963717927294531</v>
       </c>
       <c r="J23" s="1" t="n">
         <f aca="false">((J8-$J$3)/$J$3)*100</f>
@@ -26065,7 +27068,7 @@
       </c>
       <c r="K23" s="1" t="n">
         <f aca="false">((K8-$K$3)/$K$3)*100</f>
-        <v>-1.617311965189</v>
+        <v>-1.61731196518894</v>
       </c>
       <c r="N23" s="1" t="n">
         <f aca="false">((N8-$N$3)/$N$3)*100</f>
@@ -26082,11 +27085,11 @@
       </c>
       <c r="B24" s="1" t="n">
         <f aca="false">(($B$3-B10)/$B$3)*100</f>
-        <v>41.9008790177458</v>
+        <v>41.9008790177455</v>
       </c>
       <c r="C24" s="1" t="n">
         <f aca="false">(($C$3-C10)/$C$3)*100</f>
-        <v>-12.8182193321139</v>
+        <v>-12.8182193321136</v>
       </c>
       <c r="D24" s="1" t="n">
         <f aca="false">(($D$3-D10)/$D$3)*100</f>
@@ -26094,23 +27097,23 @@
       </c>
       <c r="E24" s="1" t="n">
         <f aca="false">(($E$3-E10)/$E$3)*100</f>
-        <v>-43.2601256971066</v>
+        <v>-43.2601256971072</v>
       </c>
       <c r="F24" s="1" t="n">
         <f aca="false">(($F$3-F10)/$F$3)*100</f>
-        <v>30.7033807610039</v>
+        <v>30.703380761004</v>
       </c>
       <c r="G24" s="1" t="n">
         <f aca="false">(($G$3-G10)/$G$3)*100</f>
-        <v>0.903252155130202</v>
+        <v>0.90325215513</v>
       </c>
       <c r="H24" s="1" t="n">
         <f aca="false">((H9-$H$3)/$H$3)*100</f>
-        <v>-31.9124832619592</v>
+        <v>-31.9124832619594</v>
       </c>
       <c r="J24" s="1" t="n">
         <f aca="false">((J9-$J$3)/$J$3)*100</f>
-        <v>-27.4401106337627</v>
+        <v>-27.4401106337626</v>
       </c>
       <c r="N24" s="1" t="n">
         <f aca="false">((N9-$N$3)/$N$3)*100</f>
@@ -26127,7 +27130,7 @@
       </c>
       <c r="C25" s="1" t="n">
         <f aca="false">(($C$3-C11)/$C$3)*100</f>
-        <v>24.4477106482783</v>
+        <v>24.4477106482786</v>
       </c>
       <c r="D25" s="1" t="n">
         <f aca="false">(($D$3-D11)/$D$3)*100</f>
@@ -26135,19 +27138,19 @@
       </c>
       <c r="E25" s="1" t="n">
         <f aca="false">(($E$3-E11)/$E$3)*100</f>
-        <v>3.40504394757637</v>
+        <v>3.40504394757642</v>
       </c>
       <c r="F25" s="1" t="n">
         <f aca="false">(($F$3-F11)/$F$3)*100</f>
-        <v>37.1191183050447</v>
+        <v>37.1191183050448</v>
       </c>
       <c r="G25" s="1" t="n">
         <f aca="false">(($G$3-G11)/$G$3)*100</f>
-        <v>11.7131749888473</v>
+        <v>11.7131749888471</v>
       </c>
       <c r="H25" s="1" t="n">
         <f aca="false">((H10-$H$3)/$H$3)*100</f>
-        <v>-9.36155801649742</v>
+        <v>-9.36155801649762</v>
       </c>
       <c r="I25" s="1" t="n">
         <f aca="false">((I10-$I$3)/$I$3)*100</f>
@@ -26155,19 +27158,19 @@
       </c>
       <c r="J25" s="1" t="n">
         <f aca="false">((J10-$J$3)/$J$3)*100</f>
-        <v>-6.64634944704954</v>
+        <v>-6.64634944704949</v>
       </c>
       <c r="K25" s="1" t="n">
         <f aca="false">((K10-$K$3)/$K$3)*100</f>
-        <v>9.92978607834401</v>
+        <v>9.92978607834411</v>
       </c>
       <c r="N25" s="1" t="n">
         <f aca="false">((N10-$N$3)/$N$3)*100</f>
-        <v>189.396531878877</v>
+        <v>189.396531878878</v>
       </c>
       <c r="O25" s="1" t="n">
         <f aca="false">((O10-$O$3)/$O$3)*100</f>
-        <v>86.430394101409</v>
+        <v>86.4303941014096</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26180,7 +27183,7 @@
       </c>
       <c r="C26" s="1" t="n">
         <f aca="false">(($C$3-C12)/$C$3)*100</f>
-        <v>33.7526903404649</v>
+        <v>33.7526903404647</v>
       </c>
       <c r="D26" s="1" t="n">
         <f aca="false">(($D$3-D12)/$D$3)*100</f>
@@ -26192,27 +27195,27 @@
       </c>
       <c r="F26" s="1" t="n">
         <f aca="false">(($F$3-F12)/$F$3)*100</f>
-        <v>46.5234722228645</v>
+        <v>46.5234722228646</v>
       </c>
       <c r="G26" s="1" t="n">
         <f aca="false">(($G$3-G12)/$G$3)*100</f>
-        <v>20.4948813547179</v>
+        <v>20.4948813547178</v>
       </c>
       <c r="H26" s="1" t="n">
         <f aca="false">((H11-$H$3)/$H$3)*100</f>
-        <v>11.4750977338773</v>
+        <v>11.4750977338767</v>
       </c>
       <c r="I26" s="1" t="n">
         <f aca="false">((I11-$I$3)/$I$3)*100</f>
-        <v>-2.10326826079691</v>
+        <v>-2.10326826079693</v>
       </c>
       <c r="J26" s="1" t="n">
         <f aca="false">((J11-$J$3)/$J$3)*100</f>
-        <v>3.79333694194218</v>
+        <v>3.79333694194225</v>
       </c>
       <c r="K26" s="1" t="n">
         <f aca="false">((K11-$K$3)/$K$3)*100</f>
-        <v>-0.444701621257125</v>
+        <v>-0.444701621257103</v>
       </c>
       <c r="N26" s="1" t="n">
         <f aca="false">((N11-$N$3)/$N$3)*100</f>
@@ -26245,19 +27248,19 @@
       </c>
       <c r="F27" s="1" t="n">
         <f aca="false">(($F$3-F13)/$F$3)*100</f>
-        <v>46.5794499020982</v>
+        <v>46.5794499020984</v>
       </c>
       <c r="G27" s="1" t="n">
         <f aca="false">(($G$3-G13)/$G$3)*100</f>
-        <v>24.0494193465674</v>
+        <v>24.0494193465673</v>
       </c>
       <c r="H27" s="1" t="n">
         <f aca="false">((H12-$H$3)/$H$3)*100</f>
-        <v>-2.30745301749538</v>
+        <v>-2.30745301749547</v>
       </c>
       <c r="I27" s="1" t="n">
         <f aca="false">((I12-$I$3)/$I$3)*100</f>
-        <v>15.7828789341924</v>
+        <v>15.7828789341925</v>
       </c>
       <c r="J27" s="1" t="n">
         <f aca="false">((J12-$J$3)/$J$3)*100</f>
@@ -26273,7 +27276,7 @@
       </c>
       <c r="O27" s="1" t="n">
         <f aca="false">((O12-$O$3)/$O$3)*100</f>
-        <v>605.635255509108</v>
+        <v>605.635255509109</v>
       </c>
     </row>
   </sheetData>
@@ -26294,7 +27297,7 @@
   </sheetPr>
   <dimension ref="A1:Z30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -26997,7 +28000,7 @@
   </sheetPr>
   <dimension ref="A1:Z30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -27651,7 +28654,7 @@
   </sheetPr>
   <dimension ref="A1:Z30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="AE23" activeCellId="0" sqref="AE23"/>
     </sheetView>
   </sheetViews>

</xml_diff>